<commit_message>
Added Data and Source Code from Iteration 2
The data is in its own folder. There are two zip/rar files that have the
code.
</commit_message>
<xml_diff>
--- a/Story Cards.xlsx
+++ b/Story Cards.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="122">
   <si>
     <t>User Story</t>
   </si>
@@ -52,11 +52,6 @@
   </si>
   <si>
     <t>Tasks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Create notification 
-Able to notify specific people
-</t>
   </si>
   <si>
     <t>Task Breakdown</t>
@@ -235,34 +230,14 @@
     <t>Find patterns within the data</t>
   </si>
   <si>
-    <t>Memory Context (Functional Test)</t>
-  </si>
-  <si>
     <t>Analyze data with known data</t>
-  </si>
-  <si>
-    <t>Create a database to store gait data</t>
-  </si>
-  <si>
-    <t>Query the data information</t>
-  </si>
-  <si>
-    <t>Ensure data queried matches the 
-original data</t>
   </si>
   <si>
     <t>Risk 
 (1-100)</t>
   </si>
   <si>
-    <t xml:space="preserve">Develop approaches for analysis and 
-development using tools like .net, Java, etc. </t>
-  </si>
-  <si>
     <t>Working software with tools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validate algorithm </t>
   </si>
   <si>
     <t>Obtain accelerometer data</t>
@@ -340,12 +315,231 @@
   <si>
     <t>Acceptance Test</t>
   </si>
+  <si>
+    <t>A fall is detected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Will open the notification </t>
+  </si>
+  <si>
+    <t>Collect more data</t>
+  </si>
+  <si>
+    <t>I want to see shoe data for the 
+gait pattern as a part of the 
+algorithm</t>
+  </si>
+  <si>
+    <t>Get shoe data
+Connect app via bluetooth</t>
+  </si>
+  <si>
+    <t>Collect data via bluetooth</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create notification 
+Able to notify specific people
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="4"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If fall, have time delay for automatic notification/call</t>
+    </r>
+  </si>
+  <si>
+    <t>Load phone with accelerometer data app</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apply real time accelerometer data </t>
+  </si>
+  <si>
+    <t>Able to add GPS data and other location data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automatic drop pin location </t>
+  </si>
+  <si>
+    <t>Build analysis of current data</t>
+  </si>
+  <si>
+    <t>Acceptance test</t>
+  </si>
+  <si>
+    <t>Viewable notification screen</t>
+  </si>
+  <si>
+    <t>Filter IIR (impluse response)</t>
+  </si>
+  <si>
+    <t>Speak to volunteers for obtain gait data</t>
+  </si>
+  <si>
+    <t>Data within a table for the subject</t>
+  </si>
+  <si>
+    <t>Get some amount of data (x,y,z)</t>
+  </si>
+  <si>
+    <t>Have a good presentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Embed HTML5 with Android </t>
+  </si>
+  <si>
+    <t>Pass or Fail test</t>
+  </si>
+  <si>
+    <t>Create a static equation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need notification for overall app </t>
+  </si>
+  <si>
+    <t>Risk
+(1-100)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Risk Accessment/Importance </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Similar pattern of gait </t>
+  </si>
+  <si>
+    <t>Run descriptive statistics on the data</t>
+  </si>
+  <si>
+    <t>Find functions in R to run the stats</t>
+  </si>
+  <si>
+    <t>Mean, standard deviation, median</t>
+  </si>
+  <si>
+    <t>Determine if the data is reasonable for the test set</t>
+  </si>
+  <si>
+    <t>The stats must be reasonable otherwise an algorithm will be based on unreasonable data</t>
+  </si>
+  <si>
+    <t>Place the application to read accelerometer data</t>
+  </si>
+  <si>
+    <t>Accelerometer output values will change while the phone is moving</t>
+  </si>
+  <si>
+    <t>Accelerometer output values will change according to the phone's orientation</t>
+  </si>
+  <si>
+    <t>Create android activity connections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Run application </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressing a button will connect to another activity </t>
+  </si>
+  <si>
+    <t>In order to change notification and functionalility between different sections of the app, activities must be connect to one another</t>
+  </si>
+  <si>
+    <t>Connect notification with conditions app</t>
+  </si>
+  <si>
+    <t>Make sure both sets of code can be run together</t>
+  </si>
+  <si>
+    <t>If conditions are met, the notification app will come up</t>
+  </si>
+  <si>
+    <t>All buttons work and interact with all components of the app</t>
+  </si>
+  <si>
+    <t>Velocity</t>
+  </si>
+  <si>
+    <t>Create installer for phone</t>
+  </si>
+  <si>
+    <t>Open application in phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Show application template on the phone </t>
+  </si>
+  <si>
+    <t>The application needs to be on the phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Applying the apporiate sensors from literature </t>
+  </si>
+  <si>
+    <t>Compile all recorded data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have a pattern to notify whether ranges are in or out of range </t>
+  </si>
+  <si>
+    <t>Proper analysis is needed for being the algorithm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Functionality of the app is dependent on multiple connections between activities </t>
+  </si>
+  <si>
+    <t>More data will provide a better analysis</t>
+  </si>
+  <si>
+    <t>Press send message/ after 10 second delay</t>
+  </si>
+  <si>
+    <t>A SMS message is received by correct party</t>
+  </si>
+  <si>
+    <t>The correct message is received</t>
+  </si>
+  <si>
+    <t>Important to notify concerned parties</t>
+  </si>
+  <si>
+    <t>Save message data in database</t>
+  </si>
+  <si>
+    <t>Send message notification</t>
+  </si>
+  <si>
+    <t>Set up name within a database</t>
+  </si>
+  <si>
+    <t>Set up numbers within a database</t>
+  </si>
+  <si>
+    <t>Test reponsive UI</t>
+  </si>
+  <si>
+    <t>Create UI for inputting data and input list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reduce computations of algorithm </t>
+  </si>
+  <si>
+    <t>Median changing within an interval</t>
+  </si>
+  <si>
+    <t>Creating SQLite database for data input</t>
+  </si>
+  <si>
+    <t>Impliment Algorithm in Java/Android</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,6 +550,13 @@
     <font>
       <sz val="11"/>
       <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -409,13 +610,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -697,16 +898,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
     <col min="3" max="3" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.7109375" bestFit="1" customWidth="1"/>
@@ -723,10 +924,10 @@
         <v>7</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -737,13 +938,13 @@
         <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -754,10 +955,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -768,10 +969,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -782,10 +983,10 @@
         <v>5</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -793,7 +994,40 @@
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -804,44 +1038,47 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G6"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="8.42578125" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" customWidth="1"/>
-    <col min="6" max="6" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.5703125" customWidth="1"/>
     <col min="8" max="8" width="31.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>26</v>
+      <c r="G1" s="6" t="s">
+        <v>67</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -849,19 +1086,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>120</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="D2">
         <v>100</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -869,19 +1100,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>114</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" t="s">
-        <v>39</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -889,40 +1114,27 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
       <c r="C4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D4">
-        <v>90</v>
-      </c>
-      <c r="E4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="C5">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="D5">
-        <v>100</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -930,218 +1142,302 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>116</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D6">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>113</v>
+      </c>
+      <c r="C7">
+        <v>20</v>
+      </c>
+      <c r="D7">
         <v>50</v>
       </c>
-      <c r="E6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
+      <c r="E7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H7" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="C8">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="D8">
-        <v>90</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="C9">
         <v>50</v>
       </c>
       <c r="D9">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10">
-        <v>25</v>
-      </c>
-      <c r="D10">
-        <v>100</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>121</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="D11">
         <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>50</v>
-      </c>
+      <c r="A12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C13">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="D13">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C14">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="C15">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C16">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C17">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="C18">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D18">
-        <v>85</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="C19">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="D19">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22">
+        <v>50</v>
+      </c>
+      <c r="D22">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23">
+        <v>90</v>
+      </c>
+      <c r="D23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>8</v>
       </c>
-      <c r="B20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20">
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24">
         <v>80</v>
       </c>
-      <c r="D20">
+      <c r="D24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>100</v>
+      </c>
+      <c r="B25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25">
+        <v>100</v>
+      </c>
+      <c r="D25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>100</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26">
+        <v>100</v>
+      </c>
+      <c r="D26">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A12:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1152,7 +1448,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1160,34 +1456,37 @@
     <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -1195,7 +1494,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4">
         <v>90</v>
@@ -1203,7 +1502,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5">
         <v>100</v>
@@ -1211,7 +1510,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>50</v>
@@ -1219,7 +1518,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>90</v>
@@ -1227,7 +1526,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8">
         <v>50</v>
@@ -1235,7 +1534,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B9">
         <v>100</v>
@@ -1243,7 +1542,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>100</v>
@@ -1251,7 +1550,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>50</v>
@@ -1259,7 +1558,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12">
         <v>100</v>
@@ -1267,7 +1566,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1275,7 +1574,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1283,7 +1582,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1291,7 +1590,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1299,7 +1598,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B17">
         <v>85</v>
@@ -1307,7 +1606,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B18">
         <v>100</v>
@@ -1315,7 +1614,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B19">
         <v>100</v>
@@ -1329,45 +1628,48 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="36.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="46.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="54.85546875" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:7" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="B2" s="3">
         <v>5</v>
@@ -1376,18 +1678,18 @@
         <v>100</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="3">
         <v>50</v>
@@ -1396,73 +1698,256 @@
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="3">
+        <v>60</v>
+      </c>
+      <c r="C4" s="3">
+        <v>100</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="3">
+      <c r="F4" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="3">
+        <v>10</v>
+      </c>
+      <c r="C5" s="3">
+        <v>50</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="3">
+        <f>SUM(B2:B5)</f>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="3">
+        <v>40</v>
+      </c>
+      <c r="C9" s="3">
+        <v>100</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="3">
+        <v>25</v>
+      </c>
+      <c r="C10" s="3">
+        <v>25</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="3">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3">
         <v>20</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D11" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="3">
+        <v>50</v>
+      </c>
+      <c r="C12" s="3">
+        <v>80</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" s="3" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="3">
+        <v>10</v>
+      </c>
+      <c r="C13" s="3">
+        <v>25</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="3">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3">
+        <v>25</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B15" s="3">
+        <v>25</v>
+      </c>
+      <c r="C15" s="3">
+        <v>100</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="3" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="3">
-        <v>60</v>
-      </c>
-      <c r="C5" s="3">
-        <v>100</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="3">
+      <c r="E15" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="3">
         <v>10</v>
       </c>
-      <c r="C6" s="3">
-        <v>50</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>51</v>
+      <c r="C16" s="3">
+        <v>100</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="3">
+        <f>SUM(B9:B16)</f>
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>